<commit_message>
add QALY App content, fixed
</commit_message>
<xml_diff>
--- a/myapp/Inputs/inputs.xlsx
+++ b/myapp/Inputs/inputs.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eidennay\Documents\LSHTM\covid19\COVID19_QALY_App\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juano\Dropbox\Code\Git\tbscreening_tool\myapp\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF7A3E8-4FD0-424E-AE80-B33C2D47596D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6180" activeTab="3"/>
+    <workbookView xWindow="2295" yWindow="2085" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="male_LT" sheetId="1" r:id="rId1"/>
     <sheet name="female_LT" sheetId="2" r:id="rId2"/>
     <sheet name="qol_norm" sheetId="4" r:id="rId3"/>
     <sheet name="age_covid" sheetId="3" r:id="rId4"/>
+    <sheet name="age_bands" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Age</t>
   </si>
@@ -109,22 +111,37 @@
   <si>
     <t>75+</t>
   </si>
+  <si>
+    <t>15-34</t>
+  </si>
+  <si>
+    <t>45-64</t>
+  </si>
+  <si>
+    <t>65-100</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,10 +164,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,20 +453,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="2" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -483,7 +506,7 @@
         <v>3.3355012147736913E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -503,7 +526,7 @@
         <v>3.0488727551586457E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -523,7 +546,7 @@
         <v>2.2728948922868928E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -543,7 +566,7 @@
         <v>1.7559773686957376E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -563,7 +586,7 @@
         <v>1.4098471058326208E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -583,7 +606,7 @@
         <v>1.17964870067062E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -603,7 +626,7 @@
         <v>1.0315136436683143E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -623,7 +646,7 @@
         <v>9.4526352235802316E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -643,7 +666,7 @@
         <v>9.103334325788744E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -663,7 +686,7 @@
         <v>9.239145173632458E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -683,7 +706,7 @@
         <v>9.8887984693111125E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -703,7 +726,7 @@
         <v>1.1075497099642469E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -723,7 +746,7 @@
         <v>1.2852899894834206E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -743,7 +766,7 @@
         <v>1.5302678270302865E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -763,7 +786,7 @@
         <v>1.8508551197572555E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -783,7 +806,7 @@
         <v>2.2517817009709014E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -803,7 +826,7 @@
         <v>2.7285961352202601E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -823,7 +846,7 @@
         <v>3.2607805838455928E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -843,7 +866,7 @@
         <v>3.8052523684085573E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -863,7 +886,7 @@
         <v>4.3035497695416989E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -883,7 +906,7 @@
         <v>4.7241129835084056E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -903,7 +926,7 @@
         <v>5.0527066256768414E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -923,7 +946,7 @@
         <v>5.2856515581709658E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -943,7 +966,7 @@
         <v>5.4288006965963226E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -963,7 +986,7 @@
         <v>5.495414638213925E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -983,7 +1006,7 @@
         <v>5.5036209419761443E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1003,7 +1026,7 @@
         <v>5.4740444888810456E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1023,7 +1046,7 @@
         <v>5.4280041442391952E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1043,7 +1066,7 @@
         <v>5.3864711478353105E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1063,7 +1086,7 @@
         <v>5.3698370195766581E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1083,7 +1106,7 @@
         <v>5.3984707218313575E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1103,7 +1126,7 @@
         <v>5.489860358371399E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1123,7 +1146,7 @@
         <v>5.6471814225685058E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1143,7 +1166,7 @@
         <v>5.8714966012145926E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1163,7 +1186,7 @@
         <v>6.1656554924090559E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1183,7 +1206,7 @@
         <v>6.534160517827751E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1203,7 +1226,7 @@
         <v>6.98308266286461E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1223,7 +1246,7 @@
         <v>7.5200052315480112E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1243,7 +1266,7 @@
         <v>8.153975725440503E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1263,7 +1286,7 @@
         <v>8.8954461238466883E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1283,7 +1306,7 @@
         <v>9.756180738139822E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1303,7 +1326,7 @@
         <v>1.0749108856967801E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1323,7 +1346,7 @@
         <v>1.1888097032346889E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1343,7 +1366,7 @@
         <v>1.3187613604175336E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1363,7 +1386,7 @@
         <v>1.4662256582004076E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1383,7 +1406,7 @@
         <v>1.6326116124622475E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1403,7 +1426,7 @@
         <v>1.8191945580248307E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1423,7 +1446,7 @@
         <v>2.0270121513730728E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1443,7 +1466,7 @@
         <v>2.2567384547136082E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1463,7 +1486,7 @@
         <v>2.5085370269668896E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1483,7 +1506,7 @@
         <v>2.7818963688663709E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1503,7 +1526,7 @@
         <v>3.0760282854001039E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1523,7 +1546,7 @@
         <v>3.391881733747337E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1543,7 +1566,7 @@
         <v>3.7311713566887555E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1563,7 +1586,7 @@
         <v>4.0959714753958272E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1583,7 +1606,7 @@
         <v>4.4887870748620048E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1603,7 +1626,7 @@
         <v>4.9126356736124031E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1623,7 +1646,7 @@
         <v>5.3711427957865224E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1643,7 +1666,7 @@
         <v>5.8686545478524223E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1663,7 +1686,7 @@
         <v>6.4103717768593856E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1683,7 +1706,7 @@
         <v>7.0025115114069605E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1703,7 +1726,7 @@
         <v>7.6525029404624122E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1723,7 +1746,7 @@
         <v>8.369227176811888E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1743,7 +1766,7 @@
         <v>9.163312626898467E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1763,7 +1786,7 @@
         <v>1.0047501143829948E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1783,7 +1806,7 @@
         <v>1.1037104542155392E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1803,7 +1826,7 @@
         <v>1.214948031242649E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1823,7 +1846,7 @@
         <v>1.340055670787192E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1843,7 +1866,7 @@
         <v>1.4807049176730036E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1863,7 +1886,7 @@
         <v>1.6387499062380829E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1883,7 +1906,7 @@
         <v>1.8162401370356733E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1903,7 +1926,7 @@
         <v>2.0154323751890971E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -1923,7 +1946,7 @@
         <v>2.2388010903042245E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -1943,7 +1966,7 @@
         <v>2.489046733936006E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -1963,7 +1986,7 @@
         <v>2.7691010156181042E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -1983,7 +2006,7 @@
         <v>3.0821281951554983E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2003,7 +2026,7 @@
         <v>3.4315212614492795E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -2023,7 +2046,7 @@
         <v>3.8208917224974118E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -2043,7 +2066,7 @@
         <v>4.25405159529334E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -2063,7 +2086,7 @@
         <v>4.734986068227106E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -2083,7 +2106,7 @@
         <v>5.2678152247148315E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2103,7 +2126,7 @@
         <v>5.8567431799203533E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2123,7 +2146,7 @@
         <v>6.5059930095693483E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2143,7 +2166,7 @@
         <v>7.2197259597767807E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2163,7 +2186,7 @@
         <v>8.0019436394626844E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2183,7 +2206,7 @@
         <v>8.8563722324135605E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2203,7 +2226,7 @@
         <v>9.7863282432521209E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2223,7 +2246,7 @@
         <v>0.10794565926430064</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2243,7 +2266,7 @@
         <v>0.11883107350657646</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -2263,7 +2286,7 @@
         <v>0.13053057026155271</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2283,7 +2306,7 @@
         <v>0.14304404161680509</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -2303,7 +2326,7 @@
         <v>0.1563614837270379</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -2323,7 +2346,7 @@
         <v>0.1704732516438846</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -2343,7 +2366,7 @@
         <v>0.18536269877153885</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -2363,7 +2386,7 @@
         <v>0.20100240983568257</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -2383,7 +2406,7 @@
         <v>0.21735327631486584</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -2403,7 +2426,7 @@
         <v>0.23436368016978865</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -2423,7 +2446,7 @@
         <v>0.25196882065580722</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -2443,7 +2466,7 @@
         <v>0.27009021996976162</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -2463,7 +2486,7 @@
         <v>0.28863544340130187</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -2483,7 +2506,7 @@
         <v>0.30749806836814941</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -2503,7 +2526,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -2523,7 +2546,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -2543,7 +2566,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -2563,7 +2586,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -2583,7 +2606,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -2603,7 +2626,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -2623,7 +2646,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -2643,7 +2666,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -2663,7 +2686,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -2683,7 +2706,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -2703,7 +2726,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -2723,7 +2746,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -2743,7 +2766,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -2763,7 +2786,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -2783,7 +2806,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -2803,7 +2826,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -2823,7 +2846,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -2843,7 +2866,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -2863,7 +2886,7 @@
         <v>0.40982359030090415</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -2889,21 +2912,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2923,7 +2946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2943,7 +2966,7 @@
         <v>2.9369651296826337E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2963,7 +2986,7 @@
         <v>2.7644384434394743E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2983,7 +3006,7 @@
         <v>1.7711147643617917E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3003,7 +3026,7 @@
         <v>1.266238663112896E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3023,7 +3046,7 @@
         <v>9.9624459829725763E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3043,7 +3066,7 @@
         <v>8.5064898493013711E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3063,7 +3086,7 @@
         <v>7.7735832045600889E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3083,7 +3106,7 @@
         <v>7.4977512076639295E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3103,7 +3126,7 @@
         <v>7.5271776536278291E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3123,7 +3146,7 @@
         <v>7.756702406156658E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3143,7 +3166,7 @@
         <v>8.107307695627859E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3163,7 +3186,7 @@
         <v>8.5600169335157232E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3183,7 +3206,7 @@
         <v>9.1111499780282821E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3203,7 +3226,7 @@
         <v>9.7560616076773209E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3223,7 +3246,7 @@
         <v>1.0487713192131304E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3243,7 +3266,7 @@
         <v>1.1295206169620873E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3263,7 +3286,7 @@
         <v>1.2162329851986952E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3283,7 +3306,7 @@
         <v>1.3066245400610618E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3303,7 +3326,7 @@
         <v>1.3976499838110545E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3323,7 +3346,7 @@
         <v>1.4862270528508646E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3343,7 +3366,7 @@
         <v>1.5719187650010074E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3363,7 +3386,7 @@
         <v>1.6552960819378934E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3383,7 +3406,7 @@
         <v>1.7372582503532151E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3403,7 +3426,7 @@
         <v>1.8190248848074241E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3423,7 +3446,7 @@
         <v>1.9021331496134574E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3443,7 +3466,7 @@
         <v>1.9884453498457698E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3463,7 +3486,7 @@
         <v>2.0801724018844521E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3483,7 +3506,7 @@
         <v>2.1799191241094149E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3503,7 +3526,7 @@
         <v>2.2907582940519608E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3523,7 +3546,7 @@
         <v>2.4163422278563479E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3543,7 +3566,7 @@
         <v>2.5610636024937469E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3563,7 +3586,7 @@
         <v>2.7296296629465634E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3583,7 +3606,7 @@
         <v>2.9250427707378537E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3603,7 +3626,7 @@
         <v>3.1501103482418474E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3623,7 +3646,7 @@
         <v>3.4080369634590497E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3643,7 +3666,7 @@
         <v>3.7024374991900219E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3663,7 +3686,7 @@
         <v>4.0373464056616423E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3683,7 +3706,7 @@
         <v>4.4172202795553293E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3703,7 +3726,7 @@
         <v>4.84693052836706E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3723,7 +3746,7 @@
         <v>5.3317423477398376E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3743,7 +3766,7 @@
         <v>5.8772756928759213E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3763,7 +3786,7 @@
         <v>6.4894434081127161E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3783,7 +3806,7 @@
         <v>7.1743612514279013E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3803,7 +3826,7 @@
         <v>7.9382242906268297E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3823,7 +3846,7 @@
         <v>8.7871441511241542E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3843,7 +3866,7 @@
         <v>9.7269419745729039E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3863,7 +3886,7 @@
         <v>1.07628928295342E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3883,7 +3906,7 @@
         <v>1.1899418832379532E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3903,7 +3926,7 @@
         <v>1.313973051548628E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3923,7 +3946,7 @@
         <v>1.4485419125008685E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3943,7 +3966,7 @@
         <v>1.5936006602526166E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3963,7 +3986,7 @@
         <v>1.7490875897062505E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3983,7 +4006,7 @@
         <v>1.9157838024795603E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4003,7 +4026,7 @@
         <v>2.0949007047471554E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4023,7 +4046,7 @@
         <v>2.2879236172858343E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4043,7 +4066,7 @@
         <v>2.4966626153897437E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4063,7 +4086,7 @@
         <v>2.7233131253591608E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4083,7 +4106,7 @@
         <v>2.9705290909114498E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4103,7 +4126,7 @@
         <v>3.2415123149463474E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4123,7 +4146,7 @@
         <v>3.5401226030269549E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4143,7 +4166,7 @@
         <v>3.8710146661012595E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4163,7 +4186,7 @@
         <v>4.2398094926264741E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4183,7 +4206,7 @@
         <v>4.653310226976461E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4203,7 +4226,7 @@
         <v>5.1197757022909208E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4223,7 +4246,7 @@
         <v>5.6492689638449256E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4243,7 +4266,7 @@
         <v>6.2541037915358486E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4263,7 +4286,7 @@
         <v>6.9486192807599201E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4283,7 +4306,7 @@
         <v>7.74678448930747E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4303,7 +4326,7 @@
         <v>8.6638882139277763E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4323,7 +4346,7 @@
         <v>9.7174317364654757E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4343,7 +4366,7 @@
         <v>1.092738722705203E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4363,7 +4386,7 @@
         <v>1.2316469287713178E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4383,7 +4406,7 @@
         <v>1.3910414383167279E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4403,7 +4426,7 @@
         <v>1.573826070364447E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4423,7 +4446,7 @@
         <v>1.7832618341325091E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4443,7 +4466,7 @@
         <v>2.0229916514965432E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4463,7 +4486,7 @@
         <v>2.2970610948685757E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4483,7 +4506,7 @@
         <v>2.6099330438751046E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -4503,7 +4526,7 @@
         <v>2.9664937213182349E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -4523,7 +4546,7 @@
         <v>3.3720471052875498E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -4543,7 +4566,7 @@
         <v>3.832294252727881E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -4563,7 +4586,7 @@
         <v>4.3532936422513893E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -4583,7 +4606,7 @@
         <v>4.9413982929011488E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4603,7 +4626,7 @@
         <v>5.603165194388679E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -4623,7 +4646,7 @@
         <v>6.3452325574084575E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -4643,7 +4666,7 @@
         <v>7.1741606339392014E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -4663,7 +4686,7 @@
         <v>8.0962324476212363E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4683,7 +4706,7 @@
         <v>9.1172117958426835E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4703,7 +4726,7 @@
         <v>0.10242057415317013</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4723,7 +4746,7 @@
         <v>0.11474594304200567</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -4743,7 +4766,7 @@
         <v>0.12817145902143215</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4763,7 +4786,7 @@
         <v>0.14270557561528044</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4783,7 +4806,7 @@
         <v>0.15835416654300119</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4803,7 +4826,7 @@
         <v>0.17511090322818437</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4823,7 +4846,7 @@
         <v>0.19295152804320315</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4843,7 +4866,7 @@
         <v>0.21183162495801186</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4863,7 +4886,7 @@
         <v>0.23168457214683438</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4883,7 +4906,7 @@
         <v>0.25241977490827655</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4903,7 +4926,7 @@
         <v>0.27392128371394292</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4923,7 +4946,7 @@
         <v>0.2960469050617045</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4943,7 +4966,7 @@
         <v>0.31862791122911427</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -4963,7 +4986,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -4983,7 +5006,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -5003,7 +5026,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -5023,7 +5046,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -5043,7 +5066,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -5063,7 +5086,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -5083,7 +5106,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -5103,7 +5126,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -5123,7 +5146,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -5143,7 +5166,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -5163,7 +5186,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -5183,7 +5206,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -5203,7 +5226,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -5223,7 +5246,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -5243,7 +5266,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -5263,7 +5286,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -5283,7 +5306,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -5303,7 +5326,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -5323,7 +5346,7 @@
         <v>0.43130725700263861</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -5349,19 +5372,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5387,7 +5410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -5413,7 +5436,7 @@
         <v>0.98546061111111116</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -5439,7 +5462,7 @@
         <v>0.97251985714285716</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -5465,7 +5488,7 @@
         <v>0.93993930000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -5491,7 +5514,7 @@
         <v>0.88740710000000012</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -5517,7 +5540,7 @@
         <v>0.83289360000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -5543,7 +5566,7 @@
         <v>0.78203029999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5569,7 +5592,7 @@
         <v>0.73301919999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5595,56 +5618,56 @@
         <v>0.69030099999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -5657,16 +5680,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5692,7 +5715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5718,7 +5741,7 @@
         <v>9.3023255813953494E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5744,7 +5767,7 @@
         <v>1.8604651162790699E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5770,7 +5793,7 @@
         <v>2.7906976744186047E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5796,7 +5819,7 @@
         <v>3.7209302325581397E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -5822,7 +5845,7 @@
         <v>1.3023255813953489E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5848,7 +5871,7 @@
         <v>4.3720930232558138E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -5874,7 +5897,7 @@
         <v>0.10232558139534884</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -5900,7 +5923,7 @@
         <v>0.23069767441860464</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -5926,7 +5949,7 @@
         <v>0.35627906976744184</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -5952,7 +5975,7 @@
         <v>0.24465116279069768</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5965,4 +5988,74 @@
     <ignoredError sqref="A3" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F193613-F900-4DF9-BD4B-709E8AA8F5EA}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3">
+        <v>65</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>